<commit_message>
updated mine and noone's excel sheets
</commit_message>
<xml_diff>
--- a/data-raw/submissions/Tyler Bradley - Thrones Pool.xlsx
+++ b/data-raw/submissions/Tyler Bradley - Thrones Pool.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\R\Projects\thrones-pool\data-raw\submissions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tylerbradley/Documents/thrones-pool/data-raw/submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545903E5-D25E-4711-B659-A6B025E7CF9C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B3083E-F8D4-124D-BF58-5D479AA55D09}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -262,7 +262,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -729,23 +729,23 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1928,29 +1928,29 @@
   <dimension ref="A1:IT43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1" outlineLevelCol="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" style="1" customWidth="1"/>
-    <col min="3" max="5" width="16.28515625" style="1" customWidth="1"/>
-    <col min="6" max="8" width="16.28515625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="254" width="16.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" style="1" customWidth="1"/>
+    <col min="3" max="5" width="16.33203125" style="1" customWidth="1"/>
+    <col min="6" max="8" width="16.33203125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="16.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="254" width="16.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="27.6" customHeight="1">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:8" ht="27.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-    </row>
-    <row r="2" spans="1:8" ht="20.25" customHeight="1">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+    </row>
+    <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4"/>
       <c r="B2" s="5" t="s">
         <v>1</v>
@@ -1961,7 +1961,7 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:8" ht="24.2" customHeight="1">
+    <row r="3" spans="1:8" ht="24.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="7"/>
       <c r="B3" s="29" t="s">
         <v>2</v>
@@ -1970,7 +1970,7 @@
       <c r="D3" s="30"/>
       <c r="E3" s="30"/>
     </row>
-    <row r="4" spans="1:8" ht="21.6" customHeight="1">
+    <row r="4" spans="1:8" ht="21.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="8"/>
       <c r="B4" s="9" t="s">
         <v>3</v>
@@ -1988,7 +1988,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="20.85" customHeight="1">
+    <row r="5" spans="1:8" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="8"/>
       <c r="B5" s="12" t="s">
         <v>6</v>
@@ -2012,7 +2012,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="20.85" customHeight="1">
+    <row r="6" spans="1:8" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="8"/>
       <c r="B6" s="12" t="s">
         <v>8</v>
@@ -2036,7 +2036,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="20.85" customHeight="1">
+    <row r="7" spans="1:8" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="8"/>
       <c r="B7" s="12" t="s">
         <v>10</v>
@@ -2057,7 +2057,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="20.85" customHeight="1">
+    <row r="8" spans="1:8" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="8"/>
       <c r="B8" s="12" t="s">
         <v>12</v>
@@ -2078,7 +2078,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="20.85" customHeight="1">
+    <row r="9" spans="1:8" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="8"/>
       <c r="B9" s="12" t="s">
         <v>14</v>
@@ -2096,7 +2096,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="20.85" customHeight="1">
+    <row r="10" spans="1:8" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="8"/>
       <c r="B10" s="12" t="s">
         <v>16</v>
@@ -2117,7 +2117,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="20.85" customHeight="1">
+    <row r="11" spans="1:8" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="8"/>
       <c r="B11" s="12" t="s">
         <v>18</v>
@@ -2138,7 +2138,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="20.85" customHeight="1">
+    <row r="12" spans="1:8" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="8"/>
       <c r="B12" s="12" t="s">
         <v>20</v>
@@ -2156,7 +2156,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="21" customHeight="1">
+    <row r="13" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="8"/>
       <c r="B13" s="12" t="s">
         <v>22</v>
@@ -2174,7 +2174,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="20.85" customHeight="1">
+    <row r="14" spans="1:8" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="8"/>
       <c r="B14" s="12" t="s">
         <v>24</v>
@@ -2192,7 +2192,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="20.85" customHeight="1">
+    <row r="15" spans="1:8" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="8"/>
       <c r="B15" s="12" t="s">
         <v>26</v>
@@ -2210,7 +2210,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="20.85" customHeight="1">
+    <row r="16" spans="1:8" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="8"/>
       <c r="B16" s="12" t="s">
         <v>28</v>
@@ -2228,7 +2228,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="20.85" customHeight="1">
+    <row r="17" spans="1:8" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="8"/>
       <c r="B17" s="12" t="s">
         <v>30</v>
@@ -2246,7 +2246,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="20.85" customHeight="1">
+    <row r="18" spans="1:8" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="8"/>
       <c r="B18" s="12" t="s">
         <v>32</v>
@@ -2264,7 +2264,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="20.85" customHeight="1">
+    <row r="19" spans="1:8" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="8"/>
       <c r="B19" s="12" t="s">
         <v>34</v>
@@ -2282,7 +2282,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="20.85" customHeight="1">
+    <row r="20" spans="1:8" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="8"/>
       <c r="B20" s="12" t="s">
         <v>36</v>
@@ -2300,7 +2300,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="20.85" customHeight="1">
+    <row r="21" spans="1:8" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="8"/>
       <c r="B21" s="12" t="s">
         <v>38</v>
@@ -2318,7 +2318,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="20.85" customHeight="1">
+    <row r="22" spans="1:8" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="8"/>
       <c r="B22" s="12" t="s">
         <v>40</v>
@@ -2336,13 +2336,13 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="20.85" customHeight="1">
+    <row r="23" spans="1:8" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="8"/>
       <c r="B23" s="12" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D23" s="13" t="s">
         <v>43</v>
@@ -2354,7 +2354,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="20.85" customHeight="1">
+    <row r="24" spans="1:8" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="8"/>
       <c r="B24" s="12" t="s">
         <v>44</v>
@@ -2372,7 +2372,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="24.6" customHeight="1">
+    <row r="25" spans="1:8" ht="24.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="8"/>
       <c r="B25" s="26" t="s">
         <v>46</v>
@@ -2388,13 +2388,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="20.85" customHeight="1">
+    <row r="26" spans="1:8" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="8"/>
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="23"/>
-      <c r="D26" s="24"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="22"/>
       <c r="E26" s="19" t="s">
         <v>28</v>
       </c>
@@ -2402,27 +2402,27 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="20.85" customHeight="1">
+    <row r="27" spans="1:8" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="8"/>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
       <c r="E27" s="19" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="20.85" customHeight="1">
+    <row r="28" spans="1:8" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="8"/>
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="23"/>
-      <c r="D28" s="24"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="22"/>
       <c r="E28" s="15" t="s">
         <v>7</v>
       </c>
@@ -2430,13 +2430,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="32.1" customHeight="1">
+    <row r="29" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="8"/>
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="23"/>
-      <c r="D29" s="24"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="22"/>
       <c r="E29" s="19" t="s">
         <v>6</v>
       </c>
@@ -2444,13 +2444,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="30.95" customHeight="1">
+    <row r="30" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="8"/>
-      <c r="B30" s="25" t="s">
+      <c r="B30" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="23"/>
-      <c r="D30" s="24"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="22"/>
       <c r="E30" s="19" t="s">
         <v>38</v>
       </c>
@@ -2458,13 +2458,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="29.25" customHeight="1">
+    <row r="31" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="8"/>
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
       <c r="E31" s="15" t="s">
         <v>51</v>
       </c>
@@ -2472,13 +2472,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="23.1" customHeight="1">
+    <row r="32" spans="1:8" ht="23" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="8"/>
-      <c r="B32" s="25" t="s">
+      <c r="B32" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="23"/>
-      <c r="D32" s="24"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="22"/>
       <c r="E32" s="16" t="s">
         <v>52</v>
       </c>
@@ -2486,13 +2486,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="26.25" customHeight="1">
+    <row r="33" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="8"/>
-      <c r="B33" s="25" t="s">
+      <c r="B33" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="23"/>
-      <c r="D33" s="24"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="22"/>
       <c r="E33" s="16" t="s">
         <v>53</v>
       </c>
@@ -2500,72 +2500,67 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="48.75" customHeight="1">
+    <row r="34" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="8"/>
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="23"/>
-      <c r="D34" s="24"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="22"/>
       <c r="E34" s="19" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="35" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="H35" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="36" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="H36" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="37" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="H37" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="38" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="H38" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="39" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="H39" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="40" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="H40" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="41" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="H41" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="42" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="H42" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="43" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="H43" s="3" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="B27:D27"/>
@@ -2574,6 +2569,11 @@
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="E25:G25"/>
     <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C24 E5:E24" xr:uid="{57F07D11-7A0D-8942-94C6-F3B3B20B2CAC}">

</xml_diff>